<commit_message>
Modificando APIs para foros de discusion
</commit_message>
<xml_diff>
--- a/doc/roster_ideas.xlsx
+++ b/doc/roster_ideas.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10221"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arturo/aclprojects/alumno/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43B38F4-791B-9242-960C-AAACA4E9EE95}" xr6:coauthVersionLast="30" xr6:coauthVersionMax="30" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="1280" windowWidth="28040" windowHeight="17440" xr2:uid="{2376C2F8-BDEB-E145-989B-0635E4B7770E}"/>
+    <workbookView xWindow="1580" yWindow="1100" windowWidth="28040" windowHeight="17440" xr2:uid="{2376C2F8-BDEB-E145-989B-0635E4B7770E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>code</t>
   </si>
@@ -195,13 +197,28 @@
   </si>
   <si>
     <t>group.</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>0 / 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,6 +228,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -366,10 +390,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -391,9 +416,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -705,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BE0E73-6331-5042-B30D-DFE99AEE58DE}">
-  <dimension ref="B1:AI32"/>
+  <dimension ref="B1:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH11" sqref="AH11:AI15"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,10 +817,10 @@
         <v>53</v>
       </c>
       <c r="AA4" s="15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AB4" s="15">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AC4" s="15"/>
       <c r="AD4" s="15"/>
@@ -998,7 +1025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:41" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>6</v>
       </c>
@@ -1009,7 +1036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:41" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
@@ -1048,7 +1075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
         <v>31</v>
@@ -1058,8 +1085,23 @@
         <v>21</v>
       </c>
       <c r="AA20" s="3"/>
-    </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AI20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>32</v>
@@ -1068,8 +1110,23 @@
       <c r="AA21" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>1</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
@@ -1078,8 +1135,30 @@
       <c r="AA22" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AH22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>2</v>
+      </c>
+      <c r="AK22">
+        <v>1</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22">
+        <v>1</v>
+      </c>
+      <c r="AO22">
+        <f>SUM(AI22:AM22)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
@@ -1101,12 +1180,36 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:41" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AI24">
+        <f>AI21*AI22</f>
+        <v>1</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" ref="AJ24:AM24" si="0">AJ21*AJ22</f>
+        <v>0</v>
+      </c>
+      <c r="AK24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AL24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AM24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AO24">
+        <f>SUM(AI24:AM24)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:41" x14ac:dyDescent="0.2">
       <c r="X25" t="s">
         <v>50</v>
       </c>
@@ -1114,14 +1217,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AO26" s="17">
+        <f>AO24/AO22</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="27" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>36</v>
@@ -1131,14 +1238,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>3</v>
@@ -1166,7 +1273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>38</v>
@@ -1191,9 +1298,29 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:41" x14ac:dyDescent="0.2">
       <c r="X32" t="s">
         <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6B37A-FD16-9349-996E-26133FAECFD7}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separando roster de grupo
</commit_message>
<xml_diff>
--- a/doc/roster_ideas.xlsx
+++ b/doc/roster_ideas.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arturo/aclprojects/alumno/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43B38F4-791B-9242-960C-AAACA4E9EE95}" xr6:coauthVersionLast="30" xr6:coauthVersionMax="30" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC08FB-C0EF-BB44-9ECF-AEDE3D26B4AC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1100" windowWidth="28040" windowHeight="17440" xr2:uid="{2376C2F8-BDEB-E145-989B-0635E4B7770E}"/>
+    <workbookView xWindow="3240" yWindow="1300" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{2376C2F8-BDEB-E145-989B-0635E4B7770E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
   <si>
     <t>code</t>
   </si>
@@ -212,13 +213,70 @@
   </si>
   <si>
     <t>0 / 1</t>
+  </si>
+  <si>
+    <t>Bloque</t>
+  </si>
+  <si>
+    <t>wq</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>wTotal</t>
+  </si>
+  <si>
+    <t>finalGrade</t>
+  </si>
+  <si>
+    <t>gradeQ</t>
+  </si>
+  <si>
+    <t>gradeT</t>
+  </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>FinalGradeW</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Faltaría hacer un programa que permita calcular pesos a partir de porcentajes</t>
+  </si>
+  <si>
+    <t>alumnos</t>
+  </si>
+  <si>
+    <t>alumno 1</t>
+  </si>
+  <si>
+    <t>alumno 2</t>
+  </si>
+  <si>
+    <t>alumno 3</t>
+  </si>
+  <si>
+    <t>track</t>
+  </si>
+  <si>
+    <t>quest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,8 +299,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,8 +328,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -389,12 +486,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -417,6 +595,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BE0E73-6331-5042-B30D-DFE99AEE58DE}">
   <dimension ref="B1:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="T1" zoomScale="150" workbookViewId="0">
       <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
@@ -1310,20 +1546,659 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E6B37A-FD16-9349-996E-26133FAECFD7}">
-  <dimension ref="B2"/>
+  <dimension ref="A2:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="9" width="10.83203125" style="3"/>
+    <col min="10" max="10" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="35"/>
+    </row>
+    <row r="4" spans="1:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21">
+        <f>D4+F4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
+        <f>IF(H4 &gt; 0,((D4*E4)+(F4*G4))/H4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="34">
+        <f>IF(C4&gt;0,C4*I4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="37"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="27">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
+        <v>0</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <f t="shared" ref="H5:H13" si="0">D5+F5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="31">
+        <f t="shared" ref="I5:I13" si="1">IF(H5 &gt; 0,((D5*E5)+(F5*G5))/H5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="34">
+        <f t="shared" ref="J5:J13" si="2">IF(C5&gt;0,C5*I5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="37"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="27">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="36"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="27">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="36"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="27">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19">
+        <v>2</v>
+      </c>
+      <c r="D8" s="22">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3">
+        <v>100</v>
+      </c>
+      <c r="F8" s="22">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>80</v>
+      </c>
+      <c r="H8" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="31">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="J8" s="34">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L13" si="3">I8*O8</f>
+        <v>28.5</v>
+      </c>
+      <c r="N8" s="36"/>
+      <c r="O8" s="37">
+        <v>0.3</v>
+      </c>
+      <c r="P8" s="36">
+        <f>O8*10</f>
+        <v>3</v>
+      </c>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38">
+        <f>$P$17/P8</f>
+        <v>4</v>
+      </c>
+      <c r="S8" s="36">
+        <f>R8/2</f>
+        <v>2</v>
+      </c>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="27">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>80</v>
+      </c>
+      <c r="H9" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="31">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="J9" s="34">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="N9" s="36"/>
+      <c r="O9" s="37">
+        <v>0.3</v>
+      </c>
+      <c r="P9" s="36">
+        <f>O9*10</f>
+        <v>3</v>
+      </c>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38">
+        <f>$P$17/P9</f>
+        <v>4</v>
+      </c>
+      <c r="S9" s="36">
+        <f>R9/2</f>
+        <v>2</v>
+      </c>
+      <c r="T9" s="38">
+        <f>R8+R9</f>
+        <v>8</v>
+      </c>
+      <c r="U9" s="36"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="27">
+        <v>7</v>
+      </c>
+      <c r="C10" s="19">
+        <v>0</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="36"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="27">
+        <v>8</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+      <c r="D11" s="22">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="36"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="27">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0</v>
+      </c>
+      <c r="D12" s="22">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B13" s="27">
+        <v>10</v>
+      </c>
+      <c r="C13" s="19">
+        <v>3</v>
+      </c>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>100</v>
+      </c>
+      <c r="F13" s="22">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>90</v>
+      </c>
+      <c r="H13" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="31">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="J13" s="34">
+        <f t="shared" si="2"/>
+        <v>285</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="N13" s="36"/>
+      <c r="O13" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="P13" s="36">
+        <f>O13*10</f>
+        <v>4</v>
+      </c>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38">
+        <f>(P13-P9) + (P13-P8) +R9</f>
+        <v>6</v>
+      </c>
+      <c r="S13" s="36">
+        <f>R13/2</f>
+        <v>3</v>
+      </c>
+      <c r="T13" s="36">
+        <f>O9*T9/O13</f>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="U13" s="36"/>
+    </row>
+    <row r="14" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="20">
+        <f>SUM(C4:C13)</f>
+        <v>7</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="32">
+        <f>SUM(J4:J13)/C14</f>
+        <v>90.714285714285708</v>
+      </c>
+      <c r="L14">
+        <f>SUM(L4:L13)</f>
+        <v>90.5</v>
+      </c>
+      <c r="N14" s="36"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N15" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="O15" s="37">
+        <f>MIN(O4:O13)</f>
+        <v>0.3</v>
+      </c>
+      <c r="P15" s="36">
+        <f>O15*10</f>
+        <v>3</v>
+      </c>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N16" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="O16" s="37">
+        <f>MAX(O4:O13)</f>
+        <v>0.4</v>
+      </c>
+      <c r="P16" s="36">
+        <f>O16*10</f>
+        <v>4</v>
+      </c>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N17" s="36"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="36">
+        <f>P15*P16</f>
+        <v>12</v>
+      </c>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N18" s="35"/>
+      <c r="Q18" s="35"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q19" s="35"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q20" s="35"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="Q21" s="35"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G22" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G22:L22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>